<commit_message>
I added more about string processing to workshop notebook
</commit_message>
<xml_diff>
--- a/notebooks/data/imaging_audit.xlsx
+++ b/notebooks/data/imaging_audit.xlsx
@@ -468,21 +468,21 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-06-23 13:18</t>
+          <t>2023-07-10 20:52</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-06-30 21:26</t>
+          <t>2023-07-11 00:30</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -494,21 +494,21 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2023-08-23 21:23</t>
+          <t>2023-03-16 22:25</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-09-04 22:21</t>
+          <t>2023-03-16 22:47</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -520,21 +520,21 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2023-02-27 03:15</t>
+          <t>2023-05-18 03:23</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-03-21 22:29</t>
+          <t>2023-05-18 08:19</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -546,16 +546,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023-07-05 05:48</t>
+          <t>2023-03-18 03:24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-07-21 06:28</t>
+          <t>2023-03-18 06:38</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -572,21 +572,21 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2023-05-23 19:04</t>
+          <t>2023-06-25 21:55</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-06-05 01:58</t>
+          <t>2023-06-26 14:03</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -598,16 +598,16 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2023-02-16 02:25</t>
+          <t>2023-04-24 14:54</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-02-27 06:51</t>
+          <t>2023-04-24 19:58</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -624,21 +624,21 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2023-03-31 22:14</t>
+          <t>2023-07-05 06:16</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-04-06 14:10</t>
+          <t>2023-07-05 22:47</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -650,21 +650,21 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2023-04-11 20:09</t>
+          <t>2023-04-19 13:33</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-05-07 02:54</t>
+          <t>2023-04-19 17:02</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>xr</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -676,21 +676,21 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2023-01-31 21:20</t>
+          <t>2023-05-22 17:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-02-11 05:06</t>
+          <t>2023-05-22 17:42</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>CT</t>
         </is>
       </c>
     </row>
@@ -702,21 +702,21 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2023-06-07 13:40</t>
+          <t>2023-05-13 21:50</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-06-13 17:13</t>
+          <t>2023-05-14 05:38</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -728,21 +728,21 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2023-08-19 23:04</t>
+          <t>2023-03-06 12:39</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-08-26 18:01</t>
+          <t>2023-03-06 15:33</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -754,21 +754,21 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2023-03-09 14:46</t>
+          <t>2023-04-07 09:57</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-03-26 21:14</t>
+          <t>2023-04-07 15:11</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>XRAY</t>
         </is>
       </c>
     </row>
@@ -780,16 +780,16 @@
         <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2023-03-15 22:48</t>
+          <t>2023-01-26 12:46</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-03-25 18:39</t>
+          <t>2023-01-26 14:14</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -806,21 +806,21 @@
         <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2023-03-26 18:37</t>
+          <t>2023-03-30 05:35</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-03-27 04:41</t>
+          <t>2023-03-30 06:41</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>XRAY</t>
+          <t>x-ray</t>
         </is>
       </c>
     </row>
@@ -832,21 +832,21 @@
         <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2023-08-14 19:24</t>
+          <t>2023-02-10 06:01</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2023-08-16 04:40</t>
+          <t>2023-02-10 06:11</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Ct</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -858,21 +858,21 @@
         <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2023-07-01 06:00</t>
+          <t>2023-07-30 19:28</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-07-13 15:11</t>
+          <t>2023-07-30 22:32</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>xr</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -884,21 +884,21 @@
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2023-08-20 02:57</t>
+          <t>2023-05-17 09:13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2023-08-29 23:55</t>
+          <t>2023-05-17 09:15</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>ct</t>
         </is>
       </c>
     </row>
@@ -910,21 +910,21 @@
         <v>17</v>
       </c>
       <c r="C19" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2023-06-28 05:25</t>
+          <t>2023-03-17 17:19</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2023-07-04 17:37</t>
+          <t>2023-03-17 18:56</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>Ct</t>
         </is>
       </c>
     </row>
@@ -936,21 +936,21 @@
         <v>18</v>
       </c>
       <c r="C20" t="n">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2023-08-19 03:50</t>
+          <t>2023-04-06 12:24</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2023-09-02 17:59</t>
+          <t>2023-04-07 17:05</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -962,21 +962,21 @@
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2023-08-13 01:02</t>
+          <t>2023-04-10 12:52</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2023-08-22 10:18</t>
+          <t>2023-04-10 13:17</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -988,21 +988,21 @@
         <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2023-02-24 05:06</t>
+          <t>2023-08-12 13:18</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2023-04-01 03:17</t>
+          <t>2023-08-12 13:59</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>x-ray</t>
+          <t>Ct</t>
         </is>
       </c>
     </row>
@@ -1014,21 +1014,21 @@
         <v>21</v>
       </c>
       <c r="C23" t="n">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2023-07-03 14:30</t>
+          <t>2023-06-05 17:53</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2023-07-13 22:58</t>
+          <t>2023-06-05 22:35</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Ct</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -1040,21 +1040,21 @@
         <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2023-08-22 16:06</t>
+          <t>2023-07-26 17:44</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2023-08-27 16:46</t>
+          <t>2023-07-26 18:53</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1066,21 +1066,21 @@
         <v>23</v>
       </c>
       <c r="C25" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2023-06-20 19:05</t>
+          <t>2023-07-09 04:02</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2023-06-30 15:38</t>
+          <t>2023-07-09 05:13</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1092,21 +1092,21 @@
         <v>24</v>
       </c>
       <c r="C26" t="n">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2023-07-22 03:19</t>
+          <t>2023-07-30 03:24</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2023-08-05 19:44</t>
+          <t>2023-07-30 05:22</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1118,21 +1118,21 @@
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2023-04-03 19:09</t>
+          <t>2023-08-20 21:35</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2023-04-19 18:47</t>
+          <t>2023-08-21 04:23</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>xr</t>
         </is>
       </c>
     </row>
@@ -1144,21 +1144,21 @@
         <v>26</v>
       </c>
       <c r="C28" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2023-02-10 10:24</t>
+          <t>2023-02-24 12:15</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2023-02-12 00:05</t>
+          <t>2023-02-24 15:24</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>x-ray</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -1170,21 +1170,21 @@
         <v>27</v>
       </c>
       <c r="C29" t="n">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2023-03-01 18:03</t>
+          <t>2023-05-02 13:02</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2023-03-16 06:11</t>
+          <t>2023-05-02 13:07</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>Ct</t>
         </is>
       </c>
     </row>
@@ -1196,21 +1196,21 @@
         <v>28</v>
       </c>
       <c r="C30" t="n">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2023-07-17 12:47</t>
+          <t>2023-03-09 19:03</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2023-09-09 05:26</t>
+          <t>2023-03-09 23:44</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Ct</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1222,16 +1222,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2023-03-24 18:32</t>
+          <t>2023-04-03 05:13</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2023-03-30 06:53</t>
+          <t>2023-04-03 17:55</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1248,21 +1248,21 @@
         <v>30</v>
       </c>
       <c r="C32" t="n">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2023-05-03 11:33</t>
+          <t>2023-07-06 02:02</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2023-05-04 18:44</t>
+          <t>2023-07-06 03:53</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>ct</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1274,21 +1274,21 @@
         <v>31</v>
       </c>
       <c r="C33" t="n">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2023-05-10 06:11</t>
+          <t>2023-01-25 15:22</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2023-05-27 03:40</t>
+          <t>2023-01-25 17:21</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -1300,16 +1300,16 @@
         <v>32</v>
       </c>
       <c r="C34" t="n">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2023-02-14 21:29</t>
+          <t>2023-06-12 22:36</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2023-03-01 13:28</t>
+          <t>2023-06-13 06:28</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1326,16 +1326,16 @@
         <v>33</v>
       </c>
       <c r="C35" t="n">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2023-08-20 01:56</t>
+          <t>2023-04-30 15:40</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2023-08-29 08:59</t>
+          <t>2023-05-01 02:59</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1352,21 +1352,21 @@
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2023-03-22 21:49</t>
+          <t>2023-03-17 12:12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2023-05-31 23:53</t>
+          <t>2023-03-17 12:33</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -1378,21 +1378,21 @@
         <v>35</v>
       </c>
       <c r="C37" t="n">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2023-07-12 02:26</t>
+          <t>2023-04-22 21:49</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2023-07-16 15:23</t>
+          <t>2023-04-22 22:02</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -1404,21 +1404,21 @@
         <v>36</v>
       </c>
       <c r="C38" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2023-04-16 18:16</t>
+          <t>2023-03-02 21:56</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2023-04-16 21:11</t>
+          <t>2023-03-02 23:11</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>x-ray</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -1430,21 +1430,21 @@
         <v>37</v>
       </c>
       <c r="C39" t="n">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2023-02-19 22:40</t>
+          <t>2023-01-25 11:11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2023-03-03 10:40</t>
+          <t>2023-01-25 19:13</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>ct</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1456,21 +1456,21 @@
         <v>38</v>
       </c>
       <c r="C40" t="n">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2023-02-01 07:46</t>
+          <t>2023-05-15 06:57</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2023-02-10 05:22</t>
+          <t>2023-05-15 08:01</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>XRAY</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1482,21 +1482,21 @@
         <v>39</v>
       </c>
       <c r="C41" t="n">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2023-06-11 10:26</t>
+          <t>2023-08-24 21:07</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2023-06-11 22:49</t>
+          <t>2023-08-25 07:19</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>XRAY</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1508,21 +1508,21 @@
         <v>40</v>
       </c>
       <c r="C42" t="n">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2023-04-21 00:30</t>
+          <t>2023-05-14 05:54</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2023-04-21 21:31</t>
+          <t>2023-05-14 06:19</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>ct</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1534,21 +1534,21 @@
         <v>41</v>
       </c>
       <c r="C43" t="n">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2023-02-09 20:37</t>
+          <t>2023-02-26 18:52</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2023-03-06 03:59</t>
+          <t>2023-02-26 18:52</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1560,21 +1560,21 @@
         <v>42</v>
       </c>
       <c r="C44" t="n">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2023-07-23 07:05</t>
+          <t>2023-03-25 14:14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2023-08-10 04:49</t>
+          <t>2023-03-25 14:20</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>x-ray</t>
         </is>
       </c>
     </row>
@@ -1586,21 +1586,21 @@
         <v>43</v>
       </c>
       <c r="C45" t="n">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2023-02-10 02:20</t>
+          <t>2023-04-11 10:01</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2023-02-19 15:39</t>
+          <t>2023-04-11 11:58</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1612,21 +1612,21 @@
         <v>44</v>
       </c>
       <c r="C46" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2023-05-16 05:41</t>
+          <t>2023-06-18 11:14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2023-05-17 19:59</t>
+          <t>2023-06-18 11:14</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1638,21 +1638,21 @@
         <v>45</v>
       </c>
       <c r="C47" t="n">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2023-02-26 22:35</t>
+          <t>2023-03-29 08:19</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2023-03-02 14:14</t>
+          <t>2023-03-29 09:05</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Ct</t>
+          <t>x-ray</t>
         </is>
       </c>
     </row>
@@ -1664,21 +1664,21 @@
         <v>46</v>
       </c>
       <c r="C48" t="n">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2023-06-08 04:43</t>
+          <t>2023-04-28 22:06</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2023-06-13 23:37</t>
+          <t>2023-04-28 23:45</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1690,21 +1690,21 @@
         <v>47</v>
       </c>
       <c r="C49" t="n">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2023-07-09 01:35</t>
+          <t>2023-03-31 07:48</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2023-07-10 09:54</t>
+          <t>2023-03-31 08:08</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>XRAY</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -1716,21 +1716,21 @@
         <v>48</v>
       </c>
       <c r="C50" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2023-02-19 07:42</t>
+          <t>2023-07-30 05:58</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2023-02-28 09:05</t>
+          <t>2023-07-30 10:17</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>xr</t>
         </is>
       </c>
     </row>
@@ -1742,21 +1742,21 @@
         <v>49</v>
       </c>
       <c r="C51" t="n">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2023-03-10 12:20</t>
+          <t>2023-06-15 16:01</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2023-03-18 07:02</t>
+          <t>2023-06-15 17:35</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1768,21 +1768,21 @@
         <v>50</v>
       </c>
       <c r="C52" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2023-06-01 04:15</t>
+          <t>2023-05-09 18:04</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2023-06-22 21:02</t>
+          <t>2023-05-10 16:34</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -1794,21 +1794,21 @@
         <v>51</v>
       </c>
       <c r="C53" t="n">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2023-06-21 10:34</t>
+          <t>2023-03-29 12:36</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2023-09-03 01:21</t>
+          <t>2023-03-29 14:07</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Ct</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1820,16 +1820,16 @@
         <v>52</v>
       </c>
       <c r="C54" t="n">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2023-02-17 19:54</t>
+          <t>2023-03-09 13:11</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2023-02-28 16:28</t>
+          <t>2023-03-09 13:51</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -1846,21 +1846,21 @@
         <v>53</v>
       </c>
       <c r="C55" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2023-07-15 20:35</t>
+          <t>2023-06-14 03:22</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2023-07-29 09:27</t>
+          <t>2023-06-14 04:46</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>xr</t>
         </is>
       </c>
     </row>
@@ -1872,21 +1872,21 @@
         <v>54</v>
       </c>
       <c r="C56" t="n">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2023-06-24 10:34</t>
+          <t>2023-07-06 11:54</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2023-06-25 04:55</t>
+          <t>2023-07-06 12:09</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>xr</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -1898,21 +1898,21 @@
         <v>55</v>
       </c>
       <c r="C57" t="n">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2023-06-10 04:10</t>
+          <t>2023-05-15 23:27</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2023-06-10 11:27</t>
+          <t>2023-05-16 07:01</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>XRAY</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1924,21 +1924,21 @@
         <v>56</v>
       </c>
       <c r="C58" t="n">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2023-07-24 01:01</t>
+          <t>2023-02-12 02:12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2023-08-26 07:09</t>
+          <t>2023-02-12 05:05</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -1950,21 +1950,21 @@
         <v>57</v>
       </c>
       <c r="C59" t="n">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2023-06-21 21:58</t>
+          <t>2023-05-23 22:31</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2023-06-22 07:02</t>
+          <t>2023-05-23 22:46</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -1976,16 +1976,16 @@
         <v>58</v>
       </c>
       <c r="C60" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2023-05-12 17:58</t>
+          <t>2023-08-24 08:46</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2023-05-21 16:06</t>
+          <t>2023-08-24 09:25</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2002,21 +2002,21 @@
         <v>59</v>
       </c>
       <c r="C61" t="n">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2023-07-10 20:43</t>
+          <t>2023-03-04 09:26</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2023-08-19 05:51</t>
+          <t>2023-03-04 14:29</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>xr</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -2028,21 +2028,21 @@
         <v>60</v>
       </c>
       <c r="C62" t="n">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2023-03-28 01:18</t>
+          <t>2023-06-17 17:24</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2023-04-13 08:59</t>
+          <t>2023-06-17 19:30</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -2054,21 +2054,21 @@
         <v>61</v>
       </c>
       <c r="C63" t="n">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2023-03-24 09:21</t>
+          <t>2023-06-04 04:08</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2023-03-24 18:59</t>
+          <t>2023-06-04 06:23</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Ct</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -2080,21 +2080,21 @@
         <v>62</v>
       </c>
       <c r="C64" t="n">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2023-01-25 06:07</t>
+          <t>2023-04-30 07:59</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2023-02-01 10:03</t>
+          <t>2023-04-30 15:09</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -2106,21 +2106,21 @@
         <v>63</v>
       </c>
       <c r="C65" t="n">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2023-06-05 10:22</t>
+          <t>2023-07-28 06:43</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2023-06-15 15:57</t>
+          <t>2023-07-28 10:13</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>xr</t>
         </is>
       </c>
     </row>
@@ -2132,21 +2132,21 @@
         <v>64</v>
       </c>
       <c r="C66" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2023-03-05 10:50</t>
+          <t>2023-02-01 15:08</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2023-03-05 11:31</t>
+          <t>2023-02-01 19:17</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>xr</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -2158,16 +2158,16 @@
         <v>65</v>
       </c>
       <c r="C67" t="n">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2023-07-07 04:00</t>
+          <t>2023-04-18 05:53</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2023-07-28 05:48</t>
+          <t>2023-04-18 09:44</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2184,21 +2184,21 @@
         <v>66</v>
       </c>
       <c r="C68" t="n">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2023-06-21 19:54</t>
+          <t>2023-02-05 05:25</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2023-06-30 07:57</t>
+          <t>2023-02-05 11:29</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>ct</t>
         </is>
       </c>
     </row>
@@ -2210,21 +2210,21 @@
         <v>67</v>
       </c>
       <c r="C69" t="n">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2023-02-02 07:26</t>
+          <t>2023-04-27 04:34</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2023-02-12 06:15</t>
+          <t>2023-04-27 05:42</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -2236,21 +2236,21 @@
         <v>68</v>
       </c>
       <c r="C70" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2023-05-04 10:32</t>
+          <t>2023-08-11 22:24</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2023-05-11 15:02</t>
+          <t>2023-08-11 22:54</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -2262,21 +2262,21 @@
         <v>69</v>
       </c>
       <c r="C71" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2023-05-09 00:04</t>
+          <t>2023-08-08 04:20</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2023-05-17 16:31</t>
+          <t>2023-08-08 05:43</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -2288,21 +2288,21 @@
         <v>70</v>
       </c>
       <c r="C72" t="n">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2023-04-22 19:51</t>
+          <t>2023-08-11 09:57</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2023-04-23 00:13</t>
+          <t>2023-08-11 11:47</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -2314,21 +2314,21 @@
         <v>71</v>
       </c>
       <c r="C73" t="n">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2023-04-04 18:02</t>
+          <t>2023-03-12 14:51</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2023-04-23 22:33</t>
+          <t>2023-03-12 20:06</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -2340,21 +2340,21 @@
         <v>72</v>
       </c>
       <c r="C74" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2023-05-09 12:18</t>
+          <t>2023-02-15 19:34</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2023-05-24 03:45</t>
+          <t>2023-02-15 22:25</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -2366,16 +2366,16 @@
         <v>73</v>
       </c>
       <c r="C75" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2023-05-14 17:19</t>
+          <t>2023-07-05 12:51</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2023-05-28 10:52</t>
+          <t>2023-07-05 14:07</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2392,21 +2392,21 @@
         <v>74</v>
       </c>
       <c r="C76" t="n">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2023-01-26 21:08</t>
+          <t>2023-02-22 07:28</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2023-02-01 04:17</t>
+          <t>2023-02-22 19:28</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>XRAY</t>
         </is>
       </c>
     </row>
@@ -2418,21 +2418,21 @@
         <v>75</v>
       </c>
       <c r="C77" t="n">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2023-04-21 04:37</t>
+          <t>2023-04-28 07:57</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2023-05-15 08:10</t>
+          <t>2023-04-28 09:48</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>ct</t>
+          <t>Ct</t>
         </is>
       </c>
     </row>
@@ -2444,16 +2444,16 @@
         <v>76</v>
       </c>
       <c r="C78" t="n">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2023-03-22 23:22</t>
+          <t>2023-02-06 20:17</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2023-03-30 10:37</t>
+          <t>2023-02-06 22:01</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -2470,21 +2470,21 @@
         <v>77</v>
       </c>
       <c r="C79" t="n">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2023-02-04 04:23</t>
+          <t>2023-07-29 07:33</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2023-02-15 06:23</t>
+          <t>2023-07-29 11:13</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -2496,16 +2496,16 @@
         <v>78</v>
       </c>
       <c r="C80" t="n">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2023-05-22 22:37</t>
+          <t>2023-05-17 02:45</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2023-06-03 10:40</t>
+          <t>2023-05-17 05:29</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -2522,21 +2522,21 @@
         <v>79</v>
       </c>
       <c r="C81" t="n">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2023-04-22 16:44</t>
+          <t>2023-06-15 22:20</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2023-05-05 13:25</t>
+          <t>2023-06-15 22:47</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -2548,21 +2548,21 @@
         <v>80</v>
       </c>
       <c r="C82" t="n">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2023-02-27 03:37</t>
+          <t>2023-08-04 02:41</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2023-03-18 03:58</t>
+          <t>2023-08-04 12:26</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -2574,21 +2574,21 @@
         <v>81</v>
       </c>
       <c r="C83" t="n">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2023-07-15 03:58</t>
+          <t>2023-03-30 07:53</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2023-07-26 23:03</t>
+          <t>2023-03-30 11:22</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -2600,21 +2600,21 @@
         <v>82</v>
       </c>
       <c r="C84" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2023-03-11 11:30</t>
+          <t>2023-05-11 18:11</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2023-03-19 15:20</t>
+          <t>2023-05-11 18:11</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>ct</t>
         </is>
       </c>
     </row>
@@ -2626,21 +2626,21 @@
         <v>83</v>
       </c>
       <c r="C85" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2023-04-14 13:42</t>
+          <t>2023-01-30 08:27</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2023-04-22 01:24</t>
+          <t>2023-01-30 09:24</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>XRAY</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -2652,21 +2652,21 @@
         <v>84</v>
       </c>
       <c r="C86" t="n">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2023-07-16 19:47</t>
+          <t>2023-05-07 02:29</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2023-07-25 12:00</t>
+          <t>2023-05-07 03:25</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>ct</t>
         </is>
       </c>
     </row>
@@ -2678,21 +2678,21 @@
         <v>85</v>
       </c>
       <c r="C87" t="n">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2023-08-09 22:43</t>
+          <t>2023-02-23 18:55</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2023-08-12 11:00</t>
+          <t>2023-02-24 00:41</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>x-ray</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -2704,21 +2704,21 @@
         <v>86</v>
       </c>
       <c r="C88" t="n">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2023-07-31 19:33</t>
+          <t>2023-04-07 23:05</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2023-07-31 20:50</t>
+          <t>2023-04-07 23:36</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>ct</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -2730,21 +2730,21 @@
         <v>87</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2023-04-03 13:13</t>
+          <t>2023-02-18 13:42</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2023-04-21 18:09</t>
+          <t>2023-02-18 15:11</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>x-ray</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -2756,21 +2756,21 @@
         <v>88</v>
       </c>
       <c r="C90" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2023-06-08 14:17</t>
+          <t>2023-07-22 11:58</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2023-06-16 05:48</t>
+          <t>2023-07-22 12:34</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -2782,16 +2782,16 @@
         <v>89</v>
       </c>
       <c r="C91" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2023-02-22 06:06</t>
+          <t>2023-08-10 01:04</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2023-03-18 03:28</t>
+          <t>2023-08-10 10:23</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -2808,21 +2808,21 @@
         <v>90</v>
       </c>
       <c r="C92" t="n">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2023-06-15 14:58</t>
+          <t>2023-03-28 00:11</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2023-07-17 10:02</t>
+          <t>2023-03-28 01:47</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>XRAY</t>
+          <t>mri</t>
         </is>
       </c>
     </row>
@@ -2834,21 +2834,21 @@
         <v>91</v>
       </c>
       <c r="C93" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2023-07-10 11:12</t>
+          <t>2023-07-14 14:25</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2023-07-24 01:58</t>
+          <t>2023-07-15 01:12</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -2860,21 +2860,21 @@
         <v>92</v>
       </c>
       <c r="C94" t="n">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2023-07-24 21:05</t>
+          <t>2023-07-27 06:09</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2023-08-09 08:15</t>
+          <t>2023-07-27 06:19</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>XRAY</t>
+          <t>CT</t>
         </is>
       </c>
     </row>
@@ -2886,21 +2886,21 @@
         <v>93</v>
       </c>
       <c r="C95" t="n">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2023-04-19 23:02</t>
+          <t>2023-07-06 12:16</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2023-04-21 03:17</t>
+          <t>2023-07-06 12:21</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Ct</t>
+          <t>MRI</t>
         </is>
       </c>
     </row>
@@ -2912,21 +2912,21 @@
         <v>94</v>
       </c>
       <c r="C96" t="n">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2023-07-04 13:06</t>
+          <t>2023-05-24 07:51</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2023-07-21 22:13</t>
+          <t>2023-05-24 16:54</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>CT</t>
         </is>
       </c>
     </row>
@@ -2938,21 +2938,21 @@
         <v>95</v>
       </c>
       <c r="C97" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2023-07-25 03:25</t>
+          <t>2023-05-20 21:09</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2023-08-09 10:38</t>
+          <t>2023-05-20 21:09</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Mri</t>
+          <t>xr</t>
         </is>
       </c>
     </row>
@@ -2964,21 +2964,21 @@
         <v>96</v>
       </c>
       <c r="C98" t="n">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2023-07-24 02:24</t>
+          <t>2023-05-05 03:36</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2023-08-06 03:30</t>
+          <t>2023-05-05 03:39</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>CT</t>
         </is>
       </c>
     </row>
@@ -2990,21 +2990,21 @@
         <v>97</v>
       </c>
       <c r="C99" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2023-03-12 23:49</t>
+          <t>2023-07-28 03:05</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2023-04-03 06:06</t>
+          <t>2023-07-28 07:16</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>mri</t>
+          <t>mr</t>
         </is>
       </c>
     </row>
@@ -3016,21 +3016,21 @@
         <v>98</v>
       </c>
       <c r="C100" t="n">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2023-06-11 07:29</t>
+          <t>2023-06-27 04:37</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2023-06-19 11:22</t>
+          <t>2023-06-27 06:25</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>MRI</t>
+          <t>Mri</t>
         </is>
       </c>
     </row>
@@ -3042,21 +3042,21 @@
         <v>99</v>
       </c>
       <c r="C101" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2023-05-20 11:40</t>
+          <t>2023-02-10 11:56</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2023-06-18 17:59</t>
+          <t>2023-02-10 12:12</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>mr</t>
+          <t>xr</t>
         </is>
       </c>
     </row>

</xml_diff>